<commit_message>
Updated this version with details of the COGS interface.
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="PXIPMX07 - 306SALES" sheetId="1" r:id="rId8"/>
     <sheet name="PXIPMX08 - 361DEDUCT" sheetId="8" r:id="rId9"/>
     <sheet name="PXIPMX09 - 336PCACT" sheetId="10" r:id="rId10"/>
-    <sheet name="PXIATL02 - CISATL14" sheetId="19" r:id="rId11"/>
-    <sheet name="FFLU PXIPMX08 - 361DEDUCT" sheetId="15" r:id="rId12"/>
-    <sheet name="FFLU PMXPXI01 - 325ACCRLS" sheetId="16" r:id="rId13"/>
-    <sheet name="FFLU PMXPXI02 - 331CLAIMS" sheetId="17" r:id="rId14"/>
-    <sheet name="FFLU PMXPXI03 - 359PROM" sheetId="20" r:id="rId15"/>
-    <sheet name="Formulas" sheetId="2" r:id="rId16"/>
+    <sheet name="PXIPMX10 - 336COGS" sheetId="21" r:id="rId11"/>
+    <sheet name="PXIATL02 - CISATL14" sheetId="19" r:id="rId12"/>
+    <sheet name="FFLU PXIPMX08 - 361DEDUCT" sheetId="15" r:id="rId13"/>
+    <sheet name="FFLU PMXPXI01 - 325ACCRLS" sheetId="16" r:id="rId14"/>
+    <sheet name="FFLU PMXPXI02 - 331CLAIMS" sheetId="17" r:id="rId15"/>
+    <sheet name="FFLU PMXPXI03 - 359PROM" sheetId="20" r:id="rId16"/>
+    <sheet name="Formulas" sheetId="2" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Interface Master'!$A$1:$H$30</definedName>
@@ -37,15 +38,49 @@
     <definedName name="get_date_field">Formulas!$B$22</definedName>
     <definedName name="get_numeric_field">Formulas!$B$21</definedName>
     <definedName name="numeric">Formulas!$B$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="14">'FFLU PMXPXI03 - 359PROM'!$A$1:$J$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'PXIATL02 - CISATL14'!$A$1:$L$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="15">'FFLU PMXPXI03 - 359PROM'!$A$1:$J$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">'PXIATL02 - CISATL14'!$A$1:$L$19</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Horn, Chris (Contractor)</author>
+  </authors>
+  <commentList>
+    <comment ref="F10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Actually yes but handled in the code.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="452">
   <si>
     <t>No</t>
   </si>
@@ -1392,13 +1427,22 @@
   </si>
   <si>
     <t>PromotionNumber</t>
+  </si>
+  <si>
+    <t>orderdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>S9999990.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1420,6 +1464,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2626,7 +2683,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3088,6 +3145,482 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="114.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="10">
+        <v>336003</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f t="shared" ref="M2:M11" si="0">IF(ISBLANK(H2),"",CONCATENATE(IF(LEN(H2)&lt;&gt;E2,"#",""),LEN(H2)))</f>
+        <v/>
+      </c>
+      <c r="O2" s="8" t="str">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('336003', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '336003' -&gt; RecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8">
+        <f>D2+E2</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="M3" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O3" s="8" t="str">
+        <f t="shared" ref="O3:O13" ca="1" si="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" ref="D4:D10" si="2">D3+E3</f>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O4" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O5" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(invoicenumber, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicenumber -&gt; InvoiceNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O6" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(invoicelinenumber, 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicelinenumber -&gt; InvoiceLineNumber</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="L7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O7" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(customerhierarchy, 8, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- customerhierarchy -&gt; CustomerHierarchy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="E8" s="1">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="L8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(material, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- material -&gt; Material</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O9" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.date_format(orderdate, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- orderdate -&gt; OrderDate</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>#11</v>
+      </c>
+      <c r="O10" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.numb_format(discountgiven, 'S9999990.00', pxi_common.fc_is_nullable) || -- discountgiven -&gt; DiscountGiven</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="8">
+        <f>D10+E10</f>
+        <v>72</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>500</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O11" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format('500', 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '500' -&gt; ConditionType</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" ref="D12:D13" si="3">D11+E11</f>
+        <v>82</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(currency, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- currency -&gt; Currency</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="O13" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>pxi_common.char_format(' ', 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT ' ' -&gt; PromotionNumber</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11">
     <tabColor theme="6" tint="-0.249977111117893"/>
@@ -3762,7 +4295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12">
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -5004,7 +5537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13">
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -6768,7 +7301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14">
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -8819,7 +9352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15">
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -10797,7 +11330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16">
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10966,11 +11499,11 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated the reference to the list of interfaces.
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="458">
   <si>
     <t>No</t>
   </si>
@@ -1436,6 +1436,24 @@
   </si>
   <si>
     <t>S9999990.00</t>
+  </si>
+  <si>
+    <t>PXIPMX10</t>
+  </si>
+  <si>
+    <t>336COGS</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>PXIPMX11</t>
+  </si>
+  <si>
+    <t>Cogs Extract</t>
+  </si>
+  <si>
+    <t>Cogs Reference Upload</t>
   </si>
 </sst>
 </file>
@@ -1844,11 +1862,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2664,6 +2682,55 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3151,7 +3218,7 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Updated the width of the column to handle negative numbers.
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Formats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20730" windowHeight="6480" tabRatio="635" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -1435,9 +1435,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>S9999990.00</t>
-  </si>
-  <si>
     <t>PXIPMX10</t>
   </si>
   <si>
@@ -1454,6 +1451,9 @@
   </si>
   <si>
     <t>Cogs Reference Upload</t>
+  </si>
+  <si>
+    <t>S999990.00</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1864,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
@@ -2689,7 +2689,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>220</v>
@@ -2701,10 +2701,10 @@
         <v>243</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>204</v>
@@ -2715,19 +2715,19 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>196</v>
@@ -3218,11 +3218,11 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3574,18 +3574,18 @@
         <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>#11</v>
+        <v>10</v>
       </c>
       <c r="O10" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.numb_format(discountgiven, 'S9999990.00', pxi_common.fc_is_nullable) || -- discountgiven -&gt; DiscountGiven</v>
+        <v>pxi_common.numb_format(discountgiven, 'S999990.00', pxi_common.fc_is_nullable) || -- discountgiven -&gt; DiscountGiven</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>